<commit_message>
feat: Implement React event booking application with Excel import functionality and updated mock data for testing.
</commit_message>
<xml_diff>
--- a/mock_data.xlsx
+++ b/mock_data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -507,9 +507,55 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4">
+        <v>246</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Test User 11</v>
+      </c>
+      <c r="D4" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="H4" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="I4" t="str">
+        <v>10:45 am - 11:45 am</v>
+      </c>
+      <c r="J4">
+        <v>11</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>247</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Test User 12</v>
+      </c>
+      <c r="D5" t="str">
+        <v>0987654321</v>
+      </c>
+      <c r="H5" t="str">
+        <v>2025-12-04</v>
+      </c>
+      <c r="I5" t="str">
+        <v>10:45 am - 11:45 am</v>
+      </c>
+      <c r="J5">
+        <v>12</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:K5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>